<commit_message>
added support for dataframe to png
</commit_message>
<xml_diff>
--- a/capstone_project/log_results.xlsx
+++ b/capstone_project/log_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>simname</t>
   </si>
@@ -469,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1064,6 +1064,154 @@
         <v>0.1818181818181818</v>
       </c>
     </row>
+    <row r="9" spans="1:24">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>6.538559915725273e-08</v>
+      </c>
+      <c r="E9">
+        <v>0.0002031198964687064</v>
+      </c>
+      <c r="F9">
+        <v>103</v>
+      </c>
+      <c r="G9">
+        <v>-1.947856617334764e-06</v>
+      </c>
+      <c r="H9">
+        <v>0.0002569490170571953</v>
+      </c>
+      <c r="I9">
+        <v>-0.0007576942443847656</v>
+      </c>
+      <c r="J9">
+        <v>-0.0001809597015380859</v>
+      </c>
+      <c r="K9">
+        <v>-1.311302185058594e-06</v>
+      </c>
+      <c r="L9">
+        <v>0.0001505613327026367</v>
+      </c>
+      <c r="M9">
+        <v>0.0005565881729125977</v>
+      </c>
+      <c r="N9">
+        <v>4.453056874353933e-07</v>
+      </c>
+      <c r="O9">
+        <v>6.538559915725273e-08</v>
+      </c>
+      <c r="P9">
+        <v>0.0004266728064976633</v>
+      </c>
+      <c r="Q9">
+        <v>0.0002031198964687064</v>
+      </c>
+      <c r="R9">
+        <v>3.986865858195155e-05</v>
+      </c>
+      <c r="S9">
+        <v>0.5339805825242718</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0.9636363636363636</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>6.549666409227939e-08</v>
+      </c>
+      <c r="E10">
+        <v>0.0002028722228715196</v>
+      </c>
+      <c r="F10">
+        <v>103</v>
+      </c>
+      <c r="G10">
+        <v>-2.098430741170887e-05</v>
+      </c>
+      <c r="H10">
+        <v>0.0002563086454756558</v>
+      </c>
+      <c r="I10">
+        <v>-0.0007729530334472656</v>
+      </c>
+      <c r="J10">
+        <v>-0.0001891851425170898</v>
+      </c>
+      <c r="K10">
+        <v>-2.110004425048828e-05</v>
+      </c>
+      <c r="L10">
+        <v>0.0001276731491088867</v>
+      </c>
+      <c r="M10">
+        <v>0.0005413293838500977</v>
+      </c>
+      <c r="N10">
+        <v>4.451385393622331e-07</v>
+      </c>
+      <c r="O10">
+        <v>6.549666409227939e-08</v>
+      </c>
+      <c r="P10">
+        <v>0.0004268484772183001</v>
+      </c>
+      <c r="Q10">
+        <v>0.0002028722228715196</v>
+      </c>
+      <c r="R10">
+        <v>3.986865858195155e-05</v>
+      </c>
+      <c r="S10">
+        <v>0.5242718446601942</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0.9814814814814815</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>